<commit_message>
se logro el guardado de archivos excel en el proyecto, ahora se trabaja en la forma de restar 2 archivos tipo date para obtener el tiempo de respuesta
</commit_message>
<xml_diff>
--- a/resource/reporte.xlsx
+++ b/resource/reporte.xlsx
@@ -12,18 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2019-09-17</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>01:30:37</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>AMB</t>
+  </si>
+  <si>
+    <t>SALIDA</t>
   </si>
   <si>
     <t>REGRESO</t>
@@ -66,6 +66,69 @@
   </si>
   <si>
     <t>ENTREGO</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2019-10-09</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>03:38:20</t>
+  </si>
+  <si>
+    <t>03:40:25</t>
+  </si>
+  <si>
+    <t>pendiente</t>
+  </si>
+  <si>
+    <t>Traslado</t>
+  </si>
+  <si>
+    <t>NAVAL</t>
+  </si>
+  <si>
+    <t>Calle 5</t>
+  </si>
+  <si>
+    <t>Gustavo Díaz Ordaz</t>
+  </si>
+  <si>
+    <t>Carlos Salinas de Gortari</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>03:46:05</t>
+  </si>
+  <si>
+    <t>03:48:20</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>236</t>
+  </si>
+  <si>
+    <t>04:21:28</t>
+  </si>
+  <si>
+    <t>04:24:03</t>
+  </si>
+  <si>
+    <t>MILITAR</t>
+  </si>
+  <si>
+    <t>Carlos Cruz</t>
+  </si>
+  <si>
+    <t>Felipe Calderón Hinojosa</t>
   </si>
 </sst>
 </file>
@@ -116,7 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -180,58 +243,170 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="P2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="R2" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se creo el metodo manualmente para restar 2 horas, también se modifico el metodo reportExcel para que busque mediante la union de la tabla Emergencia y Paciente, se agregaron codigo necesario para buscar mediante una fecha en el primer, segundo espacio o el segmento entre ambos
</commit_message>
<xml_diff>
--- a/resource/reporte.xlsx
+++ b/resource/reporte.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="48">
   <si>
     <t>No</t>
   </si>
@@ -68,7 +68,7 @@
     <t>ENTREGO</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>2019-10-09</t>
@@ -77,22 +77,25 @@
     <t>451</t>
   </si>
   <si>
-    <t>03:38:20</t>
-  </si>
-  <si>
-    <t>03:40:25</t>
+    <t>03:46:05</t>
+  </si>
+  <si>
+    <t>03:48:20</t>
   </si>
   <si>
     <t>pendiente</t>
   </si>
   <si>
+    <t>5R</t>
+  </si>
+  <si>
     <t>Traslado</t>
   </si>
   <si>
     <t>NAVAL</t>
   </si>
   <si>
-    <t>Calle 5</t>
+    <t>21 de Abril</t>
   </si>
   <si>
     <t>Gustavo Díaz Ordaz</t>
@@ -101,34 +104,58 @@
     <t>Carlos Salinas de Gortari</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>03:46:05</t>
-  </si>
-  <si>
-    <t>03:48:20</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>236</t>
-  </si>
-  <si>
-    <t>04:21:28</t>
-  </si>
-  <si>
-    <t>04:24:03</t>
-  </si>
-  <si>
-    <t>MILITAR</t>
-  </si>
-  <si>
-    <t>Carlos Cruz</t>
-  </si>
-  <si>
-    <t>Felipe Calderón Hinojosa</t>
+    <t>00:00:04</t>
+  </si>
+  <si>
+    <t>568</t>
+  </si>
+  <si>
+    <t>569</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>458</t>
+  </si>
+  <si>
+    <t>459</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>2019-10-10</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>11:26:36</t>
+  </si>
+  <si>
+    <t>11:29:48</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>CRUZ ROJA</t>
+  </si>
+  <si>
+    <t>Fotmando Hogar</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>452</t>
+  </si>
+  <si>
+    <t>453</t>
+  </si>
+  <si>
+    <t>454</t>
   </si>
 </sst>
 </file>
@@ -179,7 +206,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -261,7 +288,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
@@ -270,28 +297,28 @@
         <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
         <v>23</v>
@@ -299,7 +326,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -308,46 +335,46 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="R3" t="s">
         <v>23</v>
@@ -355,57 +382,281 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="N4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="P4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se realizaron la modificaciones pertinentes para que se agregará la columna de Folio y Base a la tabla EMERGENCIA, también se realizaron modificaciones para que la clase Colsulta que cree un archivo de excel con la fecha que se esta buscando. Se realizaron modificaciones a varios metodos de la clase ConxDB para que contemplen las nuevas columnas de la tabla EMERGENCIA. y se modifico el motodo reporteExcel para que las celdas sean autoajustable
</commit_message>
<xml_diff>
--- a/resource/reporte.xlsx
+++ b/resource/reporte.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="60">
   <si>
     <t>No</t>
   </si>
@@ -83,33 +83,36 @@
     <t>03:48:20</t>
   </si>
   <si>
+    <t>5R</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Traslado</t>
+  </si>
+  <si>
+    <t>NAVAL</t>
+  </si>
+  <si>
+    <t>21 de Abril</t>
+  </si>
+  <si>
+    <t>Gustavo Díaz Ordaz</t>
+  </si>
+  <si>
+    <t>Carlos Salinas de Gortari</t>
+  </si>
+  <si>
+    <t>00:00:04</t>
+  </si>
+  <si>
+    <t>568</t>
+  </si>
+  <si>
     <t>pendiente</t>
   </si>
   <si>
-    <t>5R</t>
-  </si>
-  <si>
-    <t>Traslado</t>
-  </si>
-  <si>
-    <t>NAVAL</t>
-  </si>
-  <si>
-    <t>21 de Abril</t>
-  </si>
-  <si>
-    <t>Gustavo Díaz Ordaz</t>
-  </si>
-  <si>
-    <t>Carlos Salinas de Gortari</t>
-  </si>
-  <si>
-    <t>00:00:04</t>
-  </si>
-  <si>
-    <t>568</t>
-  </si>
-  <si>
     <t>569</t>
   </si>
   <si>
@@ -156,6 +159,39 @@
   </si>
   <si>
     <t>454</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2019-10-23</t>
+  </si>
+  <si>
+    <t>951</t>
+  </si>
+  <si>
+    <t>03:01:24</t>
+  </si>
+  <si>
+    <t>03:03:01</t>
+  </si>
+  <si>
+    <t>Boca</t>
+  </si>
+  <si>
+    <t>bloqueo respiratorio</t>
+  </si>
+  <si>
+    <t>boca</t>
+  </si>
+  <si>
+    <t>00:00:08</t>
+  </si>
+  <si>
+    <t>753</t>
+  </si>
+  <si>
+    <t>754</t>
   </si>
 </sst>
 </file>
@@ -206,7 +242,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -284,17 +320,15 @@
       <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2"/>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
         <v>25</v>
@@ -302,9 +336,7 @@
       <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
+      <c r="L2"/>
       <c r="M2" t="s">
         <v>27</v>
       </c>
@@ -321,7 +353,7 @@
         <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -340,17 +372,15 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3"/>
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
@@ -358,9 +388,7 @@
       <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
+      <c r="L3"/>
       <c r="M3" t="s">
         <v>27</v>
       </c>
@@ -374,10 +402,10 @@
         <v>30</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -396,17 +424,15 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F4"/>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
@@ -414,9 +440,7 @@
       <c r="K4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
+      <c r="L4"/>
       <c r="M4" t="s">
         <v>27</v>
       </c>
@@ -430,10 +454,10 @@
         <v>30</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -452,17 +476,15 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
+      <c r="F5"/>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
         <v>25</v>
@@ -470,9 +492,7 @@
       <c r="K5" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
-        <v>23</v>
-      </c>
+      <c r="L5"/>
       <c r="M5" t="s">
         <v>27</v>
       </c>
@@ -486,51 +506,47 @@
         <v>30</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F6"/>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>23</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="L6"/>
       <c r="M6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
         <v>28</v>
@@ -539,54 +555,50 @@
         <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F7"/>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" t="s">
-        <v>23</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="L7"/>
       <c r="M7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
         <v>28</v>
@@ -595,69 +607,173 @@
         <v>29</v>
       </c>
       <c r="P7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F8"/>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s">
         <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="L8"/>
       <c r="M8" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
         <v>43</v>
       </c>
-      <c r="N8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>47</v>
-      </c>
-      <c r="R8" t="s">
-        <v>23</v>
+      <c r="L9"/>
+      <c r="M9" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>